<commit_message>
ECS reading refactor, moved to separate class
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D493F8CD-AAA3-48D9-9B34-BBE84C566B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D92D94E-A16F-46B1-99D6-412033460510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6104,7 +6104,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
Add Enterprise Project; enterpriseproj in VPC
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE8D7C-D34F-447F-9018-1DF4E7DC3A81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113633BF-1FFE-408A-8F56-BFC8EDCCFB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="234">
   <si>
     <t>group01</t>
   </si>
@@ -1593,6 +1593,12 @@
   </si>
   <si>
     <t>Copyright © Huawei Technologies Co., Ltd. 2023. All rights reserved.</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>STG</t>
   </si>
 </sst>
 </file>
@@ -2288,9 +2294,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2315,30 +2345,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2357,17 +2363,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5572,7 +5578,7 @@
   <dimension ref="A1:AO29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1"/>
@@ -5590,22 +5596,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="85"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5617,7 +5623,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="85"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5629,25 +5635,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="85"/>
+      <c r="E4" s="93"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="87"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="85"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="93"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="89"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="85"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5655,7 +5661,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="85"/>
+      <c r="E7" s="93"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5666,22 +5672,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="98" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5691,31 +5697,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5727,22 +5733,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="83" t="s">
+      <c r="A16" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="83" t="s">
+      <c r="A17" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5752,45 +5758,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="95"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5801,60 +5807,50 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="98"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="99"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="85"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5867,6 +5863,16 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -7150,17 +7156,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7168,16 +7174,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7185,16 +7191,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7202,16 +7208,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="107" t="s">
+      <c r="C5" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7219,16 +7225,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="108"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7236,16 +7242,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7253,16 +7259,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7270,16 +7276,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="107" t="s">
+      <c r="C9" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="107"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7287,16 +7293,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="107" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="107"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7304,16 +7310,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="107" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="107"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7321,16 +7327,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="107" t="s">
+      <c r="C12" s="108" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="108"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="108"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7338,16 +7344,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="108"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="107"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7355,16 +7361,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="108"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="108"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="108"/>
-      <c r="J14" s="108"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7372,16 +7378,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="107"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7389,59 +7395,67 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="C16" s="107" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="107"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="109"/>
-      <c r="J18" s="109"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7452,14 +7466,6 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -7488,7 +7494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABE4133-68EE-4AE2-AF8E-B7881ADA2847}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -7564,7 +7572,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7573,7 +7581,7 @@
     <col min="2" max="2" width="15.796875" style="76" customWidth="1"/>
     <col min="3" max="3" width="13.59765625" style="76" customWidth="1"/>
     <col min="4" max="4" width="15.3984375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.796875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.796875" style="76" customWidth="1"/>
     <col min="6" max="6" width="17.19921875" style="5" customWidth="1"/>
     <col min="7" max="16384" width="8.796875" style="5"/>
   </cols>
@@ -7591,7 +7599,7 @@
       <c r="D1" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="56" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="74" t="s">
@@ -7611,7 +7619,9 @@
       <c r="D2" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>209</v>
       </c>
@@ -7629,7 +7639,9 @@
       <c r="D3" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>210</v>
       </c>
@@ -7647,7 +7659,9 @@
       <c r="D4" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>211</v>
       </c>
@@ -7665,7 +7679,9 @@
       <c r="D5" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>212</v>
       </c>
@@ -7687,7 +7703,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Add enterpriseproj to security group
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113633BF-1FFE-408A-8F56-BFC8EDCCFB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A741A4-556E-44C0-BF95-972DFF6E2E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="229">
   <si>
     <t>group01</t>
   </si>
@@ -1278,10 +1278,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>NET</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>sa-brazil-1a</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -1298,10 +1294,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>NET01</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>10.1.1.0/24</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1314,10 +1306,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>10.4.1.0/24</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>10.1.1.1</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1330,10 +1318,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>10.4.1.1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>om-team</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1535,9 +1519,6 @@
     <t>Production</t>
   </si>
   <si>
-    <t>Inter-network</t>
-  </si>
-  <si>
     <t>Development-01</t>
   </si>
   <si>
@@ -1562,9 +1543,6 @@
     <t>10.3.0.0/16</t>
   </si>
   <si>
-    <t>10.4.0.0/16</t>
-  </si>
-  <si>
     <t>sa-brazil-1</t>
   </si>
   <si>
@@ -1599,6 +1577,9 @@
   </si>
   <si>
     <t>STG</t>
+  </si>
+  <si>
+    <t>Enterprise Project</t>
   </si>
 </sst>
 </file>
@@ -2050,7 +2031,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2294,6 +2275,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2306,9 +2320,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2321,30 +2332,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2363,17 +2350,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5596,22 +5583,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="93"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5623,7 +5610,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="93"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5635,25 +5622,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="93"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="95"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="93"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="87"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="97"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="93"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5661,7 +5648,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="93"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5672,22 +5659,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="98" t="s">
-        <v>231</v>
-      </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
+      <c r="A9" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5697,31 +5684,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5733,22 +5720,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5758,45 +5745,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5807,50 +5794,60 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="90"/>
-      <c r="B24" s="90"/>
-      <c r="C24" s="90"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="101"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="85"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="85"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5863,16 +5860,6 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -5914,34 +5901,34 @@
         <v>77</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" s="56" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>185</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>187</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5949,14 +5936,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="58" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E2" s="66" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" s="59">
         <v>30</v>
@@ -6103,7 +6090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -6164,7 +6151,7 @@
         <v>99</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>100</v>
@@ -6188,34 +6175,34 @@
         <v>119</v>
       </c>
       <c r="P1" s="78" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Q1" s="78" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="R1" s="78" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="S1" s="53" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T1" s="53" t="s">
         <v>104</v>
       </c>
       <c r="U1" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="W1" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="V1" s="53" t="s">
-        <v>202</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>203</v>
-      </c>
       <c r="X1" s="53" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="Y1" s="53" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="Z1" s="78" t="s">
         <v>105</v>
@@ -6263,7 +6250,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="70"/>
-      <c r="I2" s="110" t="s">
+      <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -6276,17 +6263,17 @@
         <v>21</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="O2" s="52"/>
       <c r="P2" s="52" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q2" s="58" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R2" s="81" t="s">
         <v>54</v>
@@ -6294,14 +6281,14 @@
       <c r="S2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="110" t="s">
+      <c r="T2" s="112" t="s">
         <v>5</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="W2" s="81" t="s">
         <v>54</v>
@@ -6309,7 +6296,7 @@
       <c r="X2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="110" t="s">
+      <c r="Y2" s="112" t="s">
         <v>19</v>
       </c>
       <c r="Z2" s="3" t="s">
@@ -6358,7 +6345,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="70"/>
-      <c r="I3" s="110"/>
+      <c r="I3" s="112"/>
       <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
@@ -6369,17 +6356,17 @@
         <v>21</v>
       </c>
       <c r="M3" s="73" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N3" s="52" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="O3" s="52"/>
       <c r="P3" s="52" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q3" s="58" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R3" s="81" t="s">
         <v>54</v>
@@ -6387,12 +6374,12 @@
       <c r="S3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="110"/>
+      <c r="T3" s="112"/>
       <c r="U3" s="55" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="W3" s="81" t="s">
         <v>54</v>
@@ -6400,7 +6387,7 @@
       <c r="X3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="110"/>
+      <c r="Y3" s="112"/>
       <c r="Z3" s="3" t="s">
         <v>6</v>
       </c>
@@ -6458,20 +6445,20 @@
         <v>22</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N4" s="52"/>
       <c r="O4" s="52" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="P4" s="52" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q4" s="58" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R4" s="81" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S4" s="73" t="s">
         <v>9</v>
@@ -6535,20 +6522,20 @@
         <v>22</v>
       </c>
       <c r="M5" s="73" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="P5" s="52" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q5" s="58" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="R5" s="81" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S5" s="73" t="s">
         <v>12</v>
@@ -7031,24 +7018,24 @@
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="103" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="103"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7">
@@ -7061,11 +7048,11 @@
       <c r="C3" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
       <c r="G3" s="51" t="s">
         <v>137</v>
       </c>
@@ -7078,36 +7065,36 @@
         <v>44890</v>
       </c>
       <c r="C4" s="54"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="54"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="54"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="54"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
       <c r="G7" s="10"/>
     </row>
   </sheetData>
@@ -7156,17 +7143,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7174,16 +7161,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="109" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7191,16 +7178,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="110" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7208,16 +7195,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="109" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7225,16 +7212,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7242,16 +7229,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="107"/>
-      <c r="J7" s="107"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7259,16 +7246,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7276,16 +7263,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="109" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7293,16 +7280,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="107" t="s">
+      <c r="C10" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7310,16 +7297,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="107" t="s">
+      <c r="C11" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="107"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7327,16 +7314,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7344,16 +7331,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="107" t="s">
+      <c r="C13" s="110" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7361,16 +7348,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="107"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7378,16 +7365,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7395,67 +7382,59 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="107" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" s="107"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
+      <c r="C16" s="110" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="106"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7466,6 +7445,14 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -7495,7 +7482,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7512,7 +7499,7 @@
         <v>77</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>78</v>
@@ -7552,12 +7539,8 @@
       <c r="D4" s="60"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="60">
-        <v>4</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>142</v>
-      </c>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
     </row>
@@ -7569,10 +7552,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF70B82-AD66-493E-91C9-92B94A95EEFB}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7591,13 +7574,13 @@
         <v>77</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>80</v>
@@ -7617,13 +7600,13 @@
         <v>52</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7637,13 +7620,13 @@
         <v>140</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -7657,33 +7640,13 @@
         <v>141</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -7700,10 +7663,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B2074E-480A-4904-B9AE-9A861A42FF00}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7721,16 +7684,16 @@
         <v>77</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F1" s="72" t="s">
         <v>82</v>
@@ -7750,16 +7713,16 @@
         <v>30</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7773,13 +7736,13 @@
         <v>30</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G3" s="50"/>
     </row>
@@ -7791,48 +7754,27 @@
         <v>141</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="13.2">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>155</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="50"/>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="13.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -7848,10 +7790,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEFA34F-B9F8-479A-9FFB-8E39D313520D}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7867,16 +7809,17 @@
     <col min="9" max="9" width="5.5" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.59765625" style="6" customWidth="1"/>
     <col min="11" max="11" width="31.19921875" style="6" customWidth="1"/>
-    <col min="12" max="13" width="8.796875" style="1"/>
-    <col min="14" max="16384" width="8.796875" style="5"/>
+    <col min="12" max="12" width="15.296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.796875" style="1"/>
+    <col min="15" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="80" customFormat="1">
+    <row r="1" spans="1:14" s="80" customFormat="1">
       <c r="A1" s="56" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C1" s="72" t="s">
         <v>83</v>
@@ -7891,10 +7834,10 @@
         <v>86</v>
       </c>
       <c r="G1" s="74" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H1" s="74" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I1" s="72" t="s">
         <v>87</v>
@@ -7905,33 +7848,36 @@
       <c r="K1" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="79"/>
+      <c r="L1" s="83" t="s">
+        <v>228</v>
+      </c>
       <c r="M1" s="79"/>
-    </row>
-    <row r="2" spans="1:13" s="80" customFormat="1">
+      <c r="N1" s="79"/>
+    </row>
+    <row r="2" spans="1:14" s="80" customFormat="1">
       <c r="A2" s="81">
         <v>1</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C2" s="81" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E2" s="82">
         <v>1</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G2" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H2" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I2" s="82" t="s">
         <v>53</v>
@@ -7942,33 +7888,36 @@
       <c r="K2" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="79"/>
+      <c r="L2" s="82" t="s">
+        <v>226</v>
+      </c>
       <c r="M2" s="79"/>
-    </row>
-    <row r="3" spans="1:13" s="80" customFormat="1">
+      <c r="N2" s="79"/>
+    </row>
+    <row r="3" spans="1:14" s="80" customFormat="1">
       <c r="A3" s="81">
         <v>2</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C3" s="81" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E3" s="82">
         <v>1</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H3" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I3" s="82" t="s">
         <v>53</v>
@@ -7979,33 +7928,36 @@
       <c r="K3" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="79"/>
+      <c r="L3" s="82" t="s">
+        <v>226</v>
+      </c>
       <c r="M3" s="79"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" s="79"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C4" s="81" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H4" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I4" s="82" t="s">
         <v>53</v>
@@ -8016,31 +7968,34 @@
       <c r="K4" s="82" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="L4" s="82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C5" s="81" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E5" s="82">
         <v>1</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G5" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I5" s="82" t="s">
         <v>53</v>
@@ -8051,31 +8006,34 @@
       <c r="K5" s="82" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="L5" s="82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C6" s="81" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E6" s="82">
         <v>1</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G6" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H6" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I6" s="82" t="s">
         <v>53</v>
@@ -8086,31 +8044,34 @@
       <c r="K6" s="82" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="L6" s="82" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C7" s="81" t="s">
         <v>56</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E7" s="82">
         <v>1</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G7" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H7" s="82" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I7" s="82" t="s">
         <v>53</v>
@@ -8121,6 +8082,23 @@
       <c r="K7" s="82" t="s">
         <v>66</v>
       </c>
+      <c r="L7" s="82" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -8157,7 +8135,7 @@
         <v>77</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>89</v>
@@ -8166,13 +8144,13 @@
         <v>80</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8180,20 +8158,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8275,40 +8253,40 @@
         <v>77</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="L1" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="M1" s="56" t="s">
         <v>171</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="L1" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8349,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8390,7 +8368,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8431,7 +8409,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:13">

</xml_diff>

<commit_message>
Add enterpriseproj to ECS and EVS
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A741A4-556E-44C0-BF95-972DFF6E2E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F009E-31D2-41AD-A2AE-146BC405D49D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="228">
   <si>
     <t>group01</t>
   </si>
@@ -768,10 +768,6 @@
   </si>
   <si>
     <t>t6.small.1</t>
-  </si>
-  <si>
-    <t>Enterprise Project Name</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Document Name</t>
@@ -5564,9 +5560,7 @@
   </sheetPr>
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
@@ -5584,7 +5578,7 @@
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="86"/>
       <c r="D1" s="86"/>
@@ -5594,7 +5588,7 @@
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
       <c r="B2" s="88" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="88"/>
       <c r="D2" s="88"/>
@@ -5604,10 +5598,10 @@
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="87"/>
@@ -5616,7 +5610,7 @@
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="21">
         <v>45024</v>
@@ -5636,7 +5630,7 @@
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="91"/>
       <c r="D6" s="18"/>
@@ -5660,7 +5654,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" s="92"/>
       <c r="C9" s="92"/>
@@ -5669,7 +5663,7 @@
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
       <c r="A10" s="93" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -5685,7 +5679,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
       <c r="A12" s="92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="92"/>
       <c r="C12" s="92"/>
@@ -5694,7 +5688,7 @@
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
       <c r="A13" s="85" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="85"/>
       <c r="C13" s="85"/>
@@ -5703,7 +5697,7 @@
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
       <c r="A14" s="85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="85"/>
       <c r="C14" s="85"/>
@@ -5712,7 +5706,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
@@ -5721,7 +5715,7 @@
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
       <c r="A16" s="85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="85"/>
       <c r="C16" s="85"/>
@@ -5730,7 +5724,7 @@
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
       <c r="A17" s="85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="85"/>
       <c r="C17" s="85"/>
@@ -5746,7 +5740,7 @@
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
       <c r="A19" s="97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="97"/>
       <c r="C19" s="97"/>
@@ -5755,10 +5749,10 @@
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="85" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" s="85" t="s">
-        <v>45</v>
       </c>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -5766,10 +5760,10 @@
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="98" t="s">
         <v>46</v>
-      </c>
-      <c r="B21" s="98" t="s">
-        <v>47</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
@@ -5777,10 +5771,10 @@
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="99" t="s">
         <v>48</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>49</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
@@ -5898,37 +5892,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>177</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5936,14 +5930,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>180</v>
       </c>
       <c r="F2" s="59">
         <v>30</v>
@@ -6011,37 +6005,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="F1" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="51" t="s">
         <v>95</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -6091,7 +6085,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6130,118 +6124,120 @@
   <sheetData>
     <row r="1" spans="1:33" ht="26.4">
       <c r="A1" s="53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="C1" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>115</v>
-      </c>
       <c r="E1" s="78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="78" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" s="53" t="s">
+      <c r="J1" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="K1" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="M1" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="S1" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="T1" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="78" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" s="78" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" s="78" t="s">
-        <v>196</v>
-      </c>
-      <c r="R1" s="78" t="s">
-        <v>202</v>
-      </c>
-      <c r="S1" s="53" t="s">
+      <c r="U1" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="V1" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="W1" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y1" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="53" t="s">
-        <v>195</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>199</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>200</v>
-      </c>
-      <c r="Y1" s="53" t="s">
-        <v>201</v>
-      </c>
-      <c r="Z1" s="78" t="s">
+      <c r="AA1" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="AA1" s="78" t="s">
+      <c r="AB1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="AD1" s="53" t="s">
+      <c r="AE1" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="AE1" s="53" t="s">
+      <c r="AF1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="AF1" s="53" t="s">
+      <c r="AG1" s="53" t="s">
         <v>111</v>
-      </c>
-      <c r="AG1" s="53" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="C2" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>20</v>
@@ -6263,20 +6259,20 @@
         <v>21</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O2" s="52"/>
       <c r="P2" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q2" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="Q2" s="58" t="s">
-        <v>211</v>
-      </c>
       <c r="R2" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>3</v>
@@ -6285,13 +6281,13 @@
         <v>5</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="W2" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>17</v>
@@ -6328,15 +6324,17 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="C3" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>20</v>
@@ -6356,33 +6354,33 @@
         <v>21</v>
       </c>
       <c r="M3" s="73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N3" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O3" s="52"/>
       <c r="P3" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q3" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" s="58" t="s">
-        <v>211</v>
-      </c>
       <c r="R3" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="T3" s="112"/>
       <c r="U3" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="W3" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>18</v>
@@ -6417,15 +6415,17 @@
       <c r="A4" s="73">
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
+      <c r="B4" s="73" t="s">
+        <v>226</v>
+      </c>
       <c r="C4" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="73" t="s">
-        <v>117</v>
-      </c>
       <c r="E4" s="73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>1</v>
@@ -6445,20 +6445,20 @@
         <v>22</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N4" s="52"/>
       <c r="O4" s="52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P4" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q4" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="Q4" s="58" t="s">
-        <v>211</v>
-      </c>
       <c r="R4" s="81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S4" s="73" t="s">
         <v>9</v>
@@ -6498,11 +6498,13 @@
       <c r="A5" s="73">
         <v>4</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="73" t="s">
+        <v>209</v>
+      </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
       <c r="E5" s="73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="73" t="s">
         <v>1</v>
@@ -6522,20 +6524,20 @@
         <v>22</v>
       </c>
       <c r="M5" s="73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P5" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q5" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="Q5" s="58" t="s">
-        <v>211</v>
-      </c>
       <c r="R5" s="81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S5" s="73" t="s">
         <v>12</v>
@@ -7016,10 +7018,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
@@ -7029,7 +7031,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="106"/>
       <c r="C2" s="106"/>
@@ -7040,26 +7042,26 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="C3" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="107" t="s">
         <v>135</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>136</v>
       </c>
       <c r="E3" s="107"/>
       <c r="F3" s="107"/>
       <c r="G3" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="9">
         <v>44890</v>
@@ -7144,7 +7146,7 @@
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
       <c r="B2" s="108" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="108"/>
       <c r="D2" s="108"/>
@@ -7162,7 +7164,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="109"/>
       <c r="E3" s="109"/>
@@ -7179,7 +7181,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="110" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="110"/>
       <c r="E4" s="110"/>
@@ -7196,7 +7198,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
@@ -7213,7 +7215,7 @@
         <v>2.1</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
@@ -7230,7 +7232,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" s="110"/>
       <c r="E7" s="110"/>
@@ -7247,7 +7249,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="110" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="110"/>
       <c r="E8" s="110"/>
@@ -7264,7 +7266,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="109" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="109"/>
       <c r="E9" s="109"/>
@@ -7281,7 +7283,7 @@
         <v>3.1</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="110"/>
       <c r="E10" s="110"/>
@@ -7298,7 +7300,7 @@
         <v>3.2</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="110"/>
       <c r="E11" s="110"/>
@@ -7315,7 +7317,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="109" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="109"/>
       <c r="E12" s="109"/>
@@ -7332,7 +7334,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C13" s="110" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="110"/>
       <c r="E13" s="110"/>
@@ -7349,7 +7351,7 @@
         <v>4.2</v>
       </c>
       <c r="C14" s="110" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="110"/>
       <c r="E14" s="110"/>
@@ -7366,7 +7368,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="109"/>
       <c r="E15" s="109"/>
@@ -7383,7 +7385,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C16" s="110" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D16" s="110"/>
       <c r="E16" s="110"/>
@@ -7496,16 +7498,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="43" customFormat="1">
       <c r="A1" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="43" customFormat="1">
@@ -7513,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -7523,7 +7525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
@@ -7533,7 +7535,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
@@ -7571,22 +7573,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="D1" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="72" t="s">
-        <v>192</v>
-      </c>
       <c r="E1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7594,19 +7596,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7614,19 +7616,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -7634,19 +7636,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -7681,25 +7683,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="71" t="s">
-        <v>192</v>
-      </c>
       <c r="F1" s="72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7707,22 +7709,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7730,19 +7732,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="50"/>
     </row>
@@ -7751,19 +7753,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>142</v>
-      </c>
       <c r="D4" s="60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7816,40 +7818,40 @@
   <sheetData>
     <row r="1" spans="1:14" s="80" customFormat="1">
       <c r="A1" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="E1" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="F1" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="G1" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>220</v>
-      </c>
-      <c r="I1" s="72" t="s">
+      <c r="J1" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="72" t="s">
-        <v>88</v>
-      </c>
       <c r="K1" s="74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="83" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M1" s="79"/>
       <c r="N1" s="79"/>
@@ -7859,37 +7861,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="82" t="s">
         <v>216</v>
-      </c>
-      <c r="C2" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>217</v>
       </c>
       <c r="E2" s="82">
         <v>1</v>
       </c>
       <c r="F2" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G2" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H2" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I2" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M2" s="79"/>
       <c r="N2" s="79"/>
@@ -7899,37 +7901,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E3" s="82">
         <v>1</v>
       </c>
       <c r="F3" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G3" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H3" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I3" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
@@ -7939,37 +7941,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="82" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>217</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
       </c>
       <c r="F4" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G4" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G4" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H4" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I4" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J4" s="82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4" s="82" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -7977,37 +7979,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="82">
         <v>1</v>
       </c>
       <c r="F5" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G5" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H5" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8015,37 +8017,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="82" t="s">
         <v>216</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="82" t="s">
-        <v>217</v>
       </c>
       <c r="E6" s="82">
         <v>1</v>
       </c>
       <c r="F6" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G6" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H6" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I6" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8053,37 +8055,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="82">
         <v>1</v>
       </c>
       <c r="F7" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G7" s="82" t="s">
         <v>221</v>
       </c>
-      <c r="G7" s="82" t="s">
-        <v>222</v>
-      </c>
       <c r="H7" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I7" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8132,25 +8134,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>155</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8158,20 +8160,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="47" t="s">
         <v>157</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8250,43 +8252,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="F1" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="L1" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="M1" s="56" t="s">
         <v>170</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8294,10 +8296,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="47">
         <v>1</v>
@@ -8306,19 +8308,19 @@
         <v>0</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="47">
         <v>0</v>
       </c>
       <c r="I2" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="47" t="s">
         <v>74</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>75</v>
       </c>
       <c r="K2" s="47">
         <v>1</v>
@@ -8327,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8335,10 +8337,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="47">
         <v>4</v>
@@ -8347,19 +8349,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="47">
         <v>0</v>
       </c>
       <c r="I3" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="47" t="s">
         <v>74</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>75</v>
       </c>
       <c r="K3" s="47">
         <v>1</v>
@@ -8368,7 +8370,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8376,10 +8378,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="47">
         <v>2</v>
@@ -8388,19 +8390,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="47">
         <v>0</v>
       </c>
       <c r="I4" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="47" t="s">
         <v>74</v>
-      </c>
-      <c r="J4" s="47" t="s">
-        <v>75</v>
       </c>
       <c r="K4" s="47">
         <v>1</v>
@@ -8409,7 +8411,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:13">

</xml_diff>

<commit_message>
Refactored servergroup deps; fix inconsistencies
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F009E-31D2-41AD-A2AE-146BC405D49D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CC54C5-2AA3-4F46-BB3C-68D61500A64A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="9" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="234">
   <si>
     <t>group01</t>
   </si>
@@ -704,15 +704,6 @@
     <t>CentOS 8.2</t>
   </si>
   <si>
-    <t>10.1.1.10</t>
-  </si>
-  <si>
-    <t>10.1.1.11</t>
-  </si>
-  <si>
-    <t>10.1.1.12</t>
-  </si>
-  <si>
     <t>SAS</t>
   </si>
   <si>
@@ -729,30 +720,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>10.1.1.21</t>
-  </si>
-  <si>
-    <t>ecs-1-01a</t>
-  </si>
-  <si>
-    <t>ecs-1-01b</t>
-  </si>
-  <si>
-    <t>ecs-1-02</t>
-  </si>
-  <si>
-    <t>ecs-1-03</t>
-  </si>
-  <si>
-    <t>10.2.1.10</t>
-  </si>
-  <si>
-    <t>10.2.1.11</t>
-  </si>
-  <si>
-    <t>10.2.1.12</t>
   </si>
   <si>
     <t>sa-brazil-1b</t>
@@ -1515,6 +1482,9 @@
     <t>Production</t>
   </si>
   <si>
+    <t>Inter-network</t>
+  </si>
+  <si>
     <t>Development-01</t>
   </si>
   <si>
@@ -1539,6 +1509,9 @@
     <t>10.3.0.0/16</t>
   </si>
   <si>
+    <t>10.4.0.0/16</t>
+  </si>
+  <si>
     <t>sa-brazil-1</t>
   </si>
   <si>
@@ -1576,6 +1549,51 @@
   </si>
   <si>
     <t>Enterprise Project</t>
+  </si>
+  <si>
+    <t>10.4.1.0/24</t>
+  </si>
+  <si>
+    <t>10.4.1.1</t>
+  </si>
+  <si>
+    <t>10.4.1.10</t>
+  </si>
+  <si>
+    <t>10.4.1.11</t>
+  </si>
+  <si>
+    <t>10.4.1.12</t>
+  </si>
+  <si>
+    <t>10.3.1.10</t>
+  </si>
+  <si>
+    <t>10.3.1.11</t>
+  </si>
+  <si>
+    <t>10.3.1.12</t>
+  </si>
+  <si>
+    <t>STG01</t>
+  </si>
+  <si>
+    <t>DEV01</t>
+  </si>
+  <si>
+    <t>10.2.1.21</t>
+  </si>
+  <si>
+    <t>ecs-prod-01a</t>
+  </si>
+  <si>
+    <t>ecs-prod-01b</t>
+  </si>
+  <si>
+    <t>ecs-dev</t>
+  </si>
+  <si>
+    <t>ecs-stg</t>
   </si>
 </sst>
 </file>
@@ -5560,7 +5578,7 @@
   </sheetPr>
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
@@ -5578,7 +5596,7 @@
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="86" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C1" s="86"/>
       <c r="D1" s="86"/>
@@ -5588,7 +5606,7 @@
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
       <c r="B2" s="88" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" s="88"/>
       <c r="D2" s="88"/>
@@ -5598,10 +5616,10 @@
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="87"/>
@@ -5610,7 +5628,7 @@
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C4" s="21">
         <v>45024</v>
@@ -5630,7 +5648,7 @@
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="90" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C6" s="91"/>
       <c r="D6" s="18"/>
@@ -5654,7 +5672,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="92" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B9" s="92"/>
       <c r="C9" s="92"/>
@@ -5663,7 +5681,7 @@
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
       <c r="A10" s="93" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -5679,7 +5697,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
       <c r="A12" s="92" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B12" s="92"/>
       <c r="C12" s="92"/>
@@ -5688,7 +5706,7 @@
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
       <c r="A13" s="85" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B13" s="85"/>
       <c r="C13" s="85"/>
@@ -5697,7 +5715,7 @@
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
       <c r="A14" s="85" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B14" s="85"/>
       <c r="C14" s="85"/>
@@ -5706,7 +5724,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
@@ -5715,7 +5733,7 @@
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
       <c r="A16" s="85" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B16" s="85"/>
       <c r="C16" s="85"/>
@@ -5724,7 +5742,7 @@
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
       <c r="A17" s="85" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B17" s="85"/>
       <c r="C17" s="85"/>
@@ -5740,7 +5758,7 @@
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
       <c r="A19" s="97" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B19" s="97"/>
       <c r="C19" s="97"/>
@@ -5749,10 +5767,10 @@
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B20" s="85" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -5760,10 +5778,10 @@
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B21" s="98" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
@@ -5771,10 +5789,10 @@
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
@@ -5892,37 +5910,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="56" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>183</v>
-      </c>
       <c r="I1" s="56" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5930,14 +5948,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="58" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E2" s="66" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F2" s="59">
         <v>30</v>
@@ -6005,37 +6023,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="51" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H1" s="51" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J1" s="51" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K1" s="51" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -6084,8 +6102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6096,7 +6114,7 @@
     <col min="4" max="4" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.09765625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.19921875" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.8984375" style="6" customWidth="1"/>
     <col min="10" max="10" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
@@ -6124,103 +6142,103 @@
   <sheetData>
     <row r="1" spans="1:33" ht="26.4">
       <c r="A1" s="53" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E1" s="78" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F1" s="78" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G1" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>184</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="T1" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="W1" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y1" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z1" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC1" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD1" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE1" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="53" t="s">
+      <c r="AF1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="AG1" s="53" t="s">
         <v>100</v>
-      </c>
-      <c r="K1" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="78" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" s="78" t="s">
-        <v>119</v>
-      </c>
-      <c r="N1" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q1" s="78" t="s">
-        <v>195</v>
-      </c>
-      <c r="R1" s="78" t="s">
-        <v>201</v>
-      </c>
-      <c r="S1" s="53" t="s">
-        <v>196</v>
-      </c>
-      <c r="T1" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="U1" s="53" t="s">
-        <v>194</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y1" s="53" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z1" s="78" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB1" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC1" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD1" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE1" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF1" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG1" s="53" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -6228,96 +6246,96 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>13</v>
+        <v>230</v>
       </c>
       <c r="H2" s="70"/>
       <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="K2" s="52" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="52" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M2" s="73" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="O2" s="52"/>
       <c r="P2" s="52" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="Q2" s="58" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="R2" s="81" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>3</v>
+        <v>224</v>
       </c>
       <c r="T2" s="112" t="s">
-        <v>5</v>
+        <v>226</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="W2" s="81" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>17</v>
+        <v>221</v>
       </c>
       <c r="Y2" s="112" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA2" s="3">
         <v>50</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC2" s="3">
         <v>1024</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AF2" s="3">
         <v>512</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -6325,90 +6343,90 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="H3" s="70"/>
       <c r="I3" s="112"/>
       <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="K3" s="52" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="52" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M3" s="73" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="N3" s="52" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="O3" s="52"/>
       <c r="P3" s="52" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="Q3" s="58" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="R3" s="81" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="T3" s="112"/>
       <c r="U3" s="55" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="W3" s="81" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="Y3" s="112"/>
       <c r="Z3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA3" s="3">
         <v>50</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC3" s="3">
         <v>1024</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AF3" s="3">
         <v>512</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:33">
@@ -6416,52 +6434,52 @@
         <v>3</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D4" s="73" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E4" s="73" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>15</v>
+        <v>232</v>
       </c>
       <c r="H4" s="70"/>
       <c r="I4" s="73"/>
       <c r="J4" s="73" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K4" s="52" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="N4" s="52"/>
       <c r="O4" s="52" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="P4" s="52" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="Q4" s="58" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="R4" s="81" t="s">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="S4" s="73" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T4" s="73"/>
       <c r="U4" s="73"/>
@@ -6470,28 +6488,28 @@
       <c r="X4" s="73"/>
       <c r="Y4" s="73"/>
       <c r="Z4" s="73" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AA4" s="73">
         <v>100</v>
       </c>
       <c r="AB4" s="73" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AC4" s="73">
         <v>512</v>
       </c>
       <c r="AD4" s="73" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="73" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AF4" s="73">
         <v>512</v>
       </c>
       <c r="AG4" s="73" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -6499,48 +6517,48 @@
         <v>4</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
       <c r="E5" s="73" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F5" s="73" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>16</v>
+        <v>233</v>
       </c>
       <c r="H5" s="70"/>
       <c r="I5" s="73"/>
       <c r="J5" s="73" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K5" s="52" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L5" s="52" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="M5" s="73" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="N5" s="52"/>
       <c r="O5" s="52" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="P5" s="52" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="Q5" s="58" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="R5" s="81" t="s">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="S5" s="73" t="s">
-        <v>12</v>
+        <v>229</v>
       </c>
       <c r="T5" s="73"/>
       <c r="U5" s="73"/>
@@ -6549,7 +6567,7 @@
       <c r="X5" s="73"/>
       <c r="Y5" s="73"/>
       <c r="Z5" s="73" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AA5" s="73">
         <v>100</v>
@@ -7018,10 +7036,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.399999999999999" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
@@ -7031,7 +7049,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="106" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B2" s="106"/>
       <c r="C2" s="106"/>
@@ -7042,26 +7060,26 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="51" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D3" s="107" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E3" s="107"/>
       <c r="F3" s="107"/>
       <c r="G3" s="51" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B4" s="9">
         <v>44890</v>
@@ -7146,7 +7164,7 @@
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
       <c r="B2" s="108" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C2" s="108"/>
       <c r="D2" s="108"/>
@@ -7164,7 +7182,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="109" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D3" s="109"/>
       <c r="E3" s="109"/>
@@ -7181,7 +7199,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="110" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D4" s="110"/>
       <c r="E4" s="110"/>
@@ -7198,7 +7216,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="109" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
@@ -7215,7 +7233,7 @@
         <v>2.1</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
@@ -7232,7 +7250,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D7" s="110"/>
       <c r="E7" s="110"/>
@@ -7249,7 +7267,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="110" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D8" s="110"/>
       <c r="E8" s="110"/>
@@ -7266,7 +7284,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="109" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D9" s="109"/>
       <c r="E9" s="109"/>
@@ -7283,7 +7301,7 @@
         <v>3.1</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D10" s="110"/>
       <c r="E10" s="110"/>
@@ -7300,7 +7318,7 @@
         <v>3.2</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D11" s="110"/>
       <c r="E11" s="110"/>
@@ -7317,7 +7335,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="109" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D12" s="109"/>
       <c r="E12" s="109"/>
@@ -7334,7 +7352,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C13" s="110" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D13" s="110"/>
       <c r="E13" s="110"/>
@@ -7351,7 +7369,7 @@
         <v>4.2</v>
       </c>
       <c r="C14" s="110" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D14" s="110"/>
       <c r="E14" s="110"/>
@@ -7368,7 +7386,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D15" s="109"/>
       <c r="E15" s="109"/>
@@ -7385,7 +7403,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C16" s="110" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D16" s="110"/>
       <c r="E16" s="110"/>
@@ -7481,10 +7499,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABE4133-68EE-4AE2-AF8E-B7881ADA2847}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7498,16 +7516,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="43" customFormat="1">
       <c r="A1" s="56" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="43" customFormat="1">
@@ -7515,7 +7533,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -7525,7 +7543,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
@@ -7535,16 +7553,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="60">
+        <v>4</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>198</v>
+      </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -7554,10 +7582,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF70B82-AD66-493E-91C9-92B94A95EEFB}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -7573,22 +7601,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="74" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F1" s="74" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7596,19 +7624,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7616,19 +7644,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -7636,20 +7664,48 @@
         <v>3</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -7665,10 +7721,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B2074E-480A-4904-B9AE-9A861A42FF00}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7683,25 +7739,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F1" s="72" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7709,22 +7765,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C2" s="66" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7732,19 +7788,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G3" s="50"/>
     </row>
@@ -7753,30 +7809,51 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="13.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>220</v>
+      </c>
       <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="13.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -7818,40 +7895,40 @@
   <sheetData>
     <row r="1" spans="1:14" s="80" customFormat="1">
       <c r="A1" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="74" t="s">
+      <c r="K1" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="83" t="s">
         <v>218</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="I1" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="83" t="s">
-        <v>227</v>
       </c>
       <c r="M1" s="79"/>
       <c r="N1" s="79"/>
@@ -7861,37 +7938,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E2" s="82">
         <v>1</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G2" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H2" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I2" s="82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J2" s="82" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M2" s="79"/>
       <c r="N2" s="79"/>
@@ -7901,37 +7978,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E3" s="82">
         <v>1</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H3" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I3" s="82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J3" s="82" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
@@ -7941,37 +8018,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H4" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I4" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="82" t="s">
-        <v>63</v>
-      </c>
       <c r="L4" s="82" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -7979,37 +8056,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E5" s="82">
         <v>1</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G5" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8017,37 +8094,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E6" s="82">
         <v>1</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G6" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H6" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I6" s="82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J6" s="82" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="L6" s="82" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8055,37 +8132,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E7" s="82">
         <v>1</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G7" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H7" s="82" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I7" s="82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8134,25 +8211,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8160,20 +8237,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8252,43 +8329,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="51" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="56" t="s">
         <v>159</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="L1" s="51" t="s">
-        <v>169</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8296,10 +8373,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D2" s="47">
         <v>1</v>
@@ -8308,19 +8385,19 @@
         <v>0</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H2" s="47">
         <v>0</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J2" s="47" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K2" s="47">
         <v>1</v>
@@ -8329,7 +8406,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8337,10 +8414,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D3" s="47">
         <v>4</v>
@@ -8349,19 +8426,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H3" s="47">
         <v>0</v>
       </c>
       <c r="I3" s="47" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J3" s="47" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K3" s="47">
         <v>1</v>
@@ -8370,7 +8447,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8378,10 +8455,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D4" s="47">
         <v>2</v>
@@ -8390,19 +8467,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H4" s="47">
         <v>0</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K4" s="47">
         <v>1</v>
@@ -8411,7 +8488,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="65" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:13">

</xml_diff>

<commit_message>
Fix ECS OS password
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CC54C5-2AA3-4F46-BB3C-68D61500A64A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD9ADF-7DDE-4BAE-ABF1-163EB076AF73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="9" r:id="rId1"/>
@@ -2295,9 +2295,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2322,30 +2346,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2364,17 +2364,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5578,7 +5578,7 @@
   </sheetPr>
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
@@ -5595,22 +5595,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="87"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="87"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="95"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5622,7 +5622,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="87"/>
+      <c r="E3" s="95"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5634,25 +5634,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="87"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="87"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="95"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="91"/>
+      <c r="C6" s="99"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="87"/>
+      <c r="E6" s="95"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5660,7 +5660,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="87"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5671,22 +5671,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5696,31 +5696,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5732,22 +5732,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5757,45 +5757,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5806,60 +5806,50 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="100"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="100"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5872,6 +5862,16 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6102,8 +6102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6120,7 +6120,7 @@
     <col min="10" max="10" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.59765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.09765625" style="6" customWidth="1"/>
     <col min="14" max="14" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
@@ -7163,17 +7163,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7181,16 +7181,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7198,16 +7198,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7215,16 +7215,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7232,16 +7232,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7249,16 +7249,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7266,16 +7266,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7283,16 +7283,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7300,16 +7300,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="110" t="s">
+      <c r="C10" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7317,16 +7317,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="109" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7334,16 +7334,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="109"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7351,16 +7351,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7368,16 +7368,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7385,16 +7385,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7402,59 +7402,67 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="110" t="s">
+      <c r="C16" s="109" t="s">
         <v>214</v>
       </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7465,14 +7473,6 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Add ECS keypair support
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD9ADF-7DDE-4BAE-ABF1-163EB076AF73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789DDF65-F04F-4CA6-9783-65FACC2EFCEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="231">
   <si>
     <t>group01</t>
   </si>
@@ -1153,10 +1153,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Password or Keypair </t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Project / IAM </t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1414,12 +1410,6 @@
   </si>
   <si>
     <t>Wave</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>keypair</t>
   </si>
   <si>
     <t>NIC1 VPC</t>
@@ -1937,7 +1927,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2010,6 +2000,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2045,7 +2048,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2376,7 +2379,10 @@
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5672,7 +5678,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="100" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B9" s="100"/>
       <c r="C9" s="100"/>
@@ -5913,34 +5919,34 @@
         <v>65</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>165</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>169</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5948,14 +5954,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>167</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>168</v>
       </c>
       <c r="F2" s="59">
         <v>30</v>
@@ -6100,10 +6106,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6120,32 +6126,31 @@
     <col min="10" max="10" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.59765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.09765625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.3984375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="18.796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.59765625" style="6" customWidth="1"/>
-    <col min="20" max="21" width="16.69921875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="12.3984375" style="6" customWidth="1"/>
-    <col min="23" max="23" width="18.796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.69921875" style="6" customWidth="1"/>
-    <col min="25" max="25" width="12.5" style="6" customWidth="1"/>
-    <col min="26" max="26" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="8.796875" style="6"/>
-    <col min="31" max="32" width="8.796875" style="1"/>
-    <col min="33" max="33" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.796875" style="1"/>
+    <col min="13" max="13" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.3984375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="18.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.59765625" style="6" customWidth="1"/>
+    <col min="19" max="20" width="16.69921875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="12.3984375" style="6" customWidth="1"/>
+    <col min="22" max="22" width="18.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.69921875" style="6" customWidth="1"/>
+    <col min="24" max="24" width="12.5" style="6" customWidth="1"/>
+    <col min="25" max="25" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="8.796875" style="6"/>
+    <col min="30" max="31" width="8.796875" style="1"/>
+    <col min="32" max="32" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="26.4">
+    <row r="1" spans="1:32" ht="26.4">
       <c r="A1" s="53" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" s="53" t="s">
         <v>102</v>
@@ -6163,7 +6168,7 @@
         <v>87</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>88</v>
@@ -6178,75 +6183,72 @@
         <v>91</v>
       </c>
       <c r="M1" s="78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N1" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="53" t="s">
         <v>107</v>
       </c>
+      <c r="O1" s="78" t="s">
+        <v>173</v>
+      </c>
       <c r="P1" s="78" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="Q1" s="78" t="s">
-        <v>184</v>
-      </c>
-      <c r="R1" s="78" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="R1" s="53" t="s">
+        <v>182</v>
       </c>
       <c r="S1" s="53" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
       <c r="T1" s="53" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="U1" s="53" t="s">
         <v>183</v>
       </c>
       <c r="V1" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="W1" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="X1" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="W1" s="53" t="s">
-        <v>187</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y1" s="53" t="s">
-        <v>189</v>
+      <c r="Y1" s="78" t="s">
+        <v>93</v>
       </c>
       <c r="Z1" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="78" t="s">
         <v>94</v>
       </c>
+      <c r="AA1" s="53" t="s">
+        <v>95</v>
+      </c>
       <c r="AB1" s="53" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AC1" s="53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AD1" s="53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AE1" s="53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF1" s="53" t="s">
-        <v>99</v>
-      </c>
-      <c r="AG1" s="53" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:32">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>104</v>
@@ -6261,7 +6263,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H2" s="70"/>
       <c r="I2" s="112" t="s">
@@ -6276,74 +6278,71 @@
       <c r="L2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="N2" s="52" t="s">
-        <v>191</v>
-      </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="R2" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="T2" s="112" t="s">
-        <v>226</v>
-      </c>
-      <c r="U2" s="55" t="s">
+      <c r="M2" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q2" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="S2" s="112" t="s">
+        <v>223</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="W2" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y2" s="112" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="V2" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="X2" s="112" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="Z2" s="3">
         <v>50</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AB2" s="3">
         <v>1024</v>
       </c>
+      <c r="AC2" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="AD2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AE2" s="3">
         <v>512</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:32">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>104</v>
@@ -6358,10 +6357,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H3" s="70"/>
-      <c r="I3" s="112"/>
+      <c r="I3" s="113"/>
       <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
@@ -6371,70 +6370,67 @@
       <c r="L3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="N3" s="52" t="s">
-        <v>191</v>
-      </c>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q3" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="R3" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="T3" s="112"/>
-      <c r="U3" s="55" t="s">
+      <c r="M3" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="P3" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q3" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="S3" s="113"/>
+      <c r="T3" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="U3" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="75" t="s">
-        <v>201</v>
-      </c>
-      <c r="W3" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="3" t="s">
+      <c r="V3" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="X3" s="113"/>
+      <c r="Y3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="Z3" s="3">
         <v>50</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AB3" s="3">
         <v>1024</v>
       </c>
+      <c r="AC3" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="AD3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AE3" s="3">
         <v>512</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:32">
       <c r="A4" s="73">
         <v>3</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>104</v>
@@ -6449,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H4" s="70"/>
       <c r="I4" s="73"/>
@@ -6462,62 +6458,61 @@
       <c r="L4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="73" t="s">
-        <v>175</v>
-      </c>
-      <c r="N4" s="52"/>
+      <c r="M4" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="N4" s="52" t="s">
+        <v>189</v>
+      </c>
       <c r="O4" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="P4" s="52" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q4" s="58" t="s">
-        <v>228</v>
-      </c>
-      <c r="R4" s="81" t="s">
+        <v>213</v>
+      </c>
+      <c r="P4" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q4" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="73" t="s">
+      <c r="R4" s="73" t="s">
         <v>6</v>
       </c>
+      <c r="S4" s="73"/>
       <c r="T4" s="73"/>
       <c r="U4" s="73"/>
       <c r="V4" s="73"/>
       <c r="W4" s="73"/>
       <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73" t="s">
+      <c r="Y4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="73">
+      <c r="Z4" s="73">
         <v>100</v>
       </c>
-      <c r="AB4" s="73" t="s">
+      <c r="AA4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" s="73">
+      <c r="AB4" s="73">
         <v>512</v>
       </c>
+      <c r="AC4" s="73" t="s">
+        <v>8</v>
+      </c>
       <c r="AD4" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="73">
+        <v>512</v>
+      </c>
+      <c r="AF4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="AE4" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF4" s="73">
-        <v>512</v>
-      </c>
-      <c r="AG4" s="73" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33">
+    </row>
+    <row r="5" spans="1:32">
       <c r="A5" s="73">
         <v>4</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
@@ -6528,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H5" s="70"/>
       <c r="I5" s="73"/>
@@ -6541,45 +6536,44 @@
       <c r="L5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="73" t="s">
-        <v>175</v>
-      </c>
-      <c r="N5" s="52"/>
+      <c r="M5" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="N5" s="52" t="s">
+        <v>189</v>
+      </c>
       <c r="O5" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="P5" s="52" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q5" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="R5" s="81" t="s">
+        <v>214</v>
+      </c>
+      <c r="P5" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q5" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="73" t="s">
-        <v>229</v>
-      </c>
+      <c r="R5" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="S5" s="73"/>
       <c r="T5" s="73"/>
       <c r="U5" s="73"/>
       <c r="V5" s="73"/>
       <c r="W5" s="73"/>
       <c r="X5" s="73"/>
-      <c r="Y5" s="73"/>
-      <c r="Z5" s="73" t="s">
+      <c r="Y5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="73">
+      <c r="Z5" s="73">
         <v>100</v>
       </c>
+      <c r="AA5" s="73"/>
       <c r="AB5" s="73"/>
       <c r="AC5" s="73"/>
-      <c r="AD5" s="73"/>
+      <c r="AD5" s="52"/>
       <c r="AE5" s="52"/>
       <c r="AF5" s="52"/>
-      <c r="AG5" s="52"/>
-    </row>
-    <row r="6" spans="1:33">
+    </row>
+    <row r="6" spans="1:32">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="52"/>
@@ -6592,15 +6586,15 @@
       <c r="J6" s="3"/>
       <c r="K6" s="52"/>
       <c r="L6" s="52"/>
-      <c r="M6" s="73"/>
+      <c r="M6" s="52"/>
       <c r="N6" s="52"/>
       <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
+      <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="55"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -6609,12 +6603,11 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
+      <c r="AD6" s="52"/>
       <c r="AE6" s="52"/>
       <c r="AF6" s="52"/>
-      <c r="AG6" s="52"/>
-    </row>
-    <row r="7" spans="1:33">
+    </row>
+    <row r="7" spans="1:32">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="52"/>
@@ -6627,15 +6620,15 @@
       <c r="J7" s="3"/>
       <c r="K7" s="52"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="73"/>
+      <c r="M7" s="52"/>
       <c r="N7" s="52"/>
       <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="55"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -6644,12 +6637,11 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
+      <c r="AD7" s="52"/>
       <c r="AE7" s="52"/>
       <c r="AF7" s="52"/>
-      <c r="AG7" s="52"/>
-    </row>
-    <row r="8" spans="1:33">
+    </row>
+    <row r="8" spans="1:32">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="52"/>
@@ -6662,15 +6654,15 @@
       <c r="J8" s="3"/>
       <c r="K8" s="52"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="73"/>
+      <c r="M8" s="52"/>
       <c r="N8" s="52"/>
       <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
+      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -6679,12 +6671,11 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
+      <c r="AD8" s="52"/>
       <c r="AE8" s="52"/>
       <c r="AF8" s="52"/>
-      <c r="AG8" s="52"/>
-    </row>
-    <row r="9" spans="1:33">
+    </row>
+    <row r="9" spans="1:32">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="52"/>
@@ -6697,15 +6688,15 @@
       <c r="J9" s="3"/>
       <c r="K9" s="52"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="73"/>
+      <c r="M9" s="52"/>
       <c r="N9" s="52"/>
       <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -6714,12 +6705,11 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
+      <c r="AD9" s="52"/>
       <c r="AE9" s="52"/>
       <c r="AF9" s="52"/>
-      <c r="AG9" s="52"/>
-    </row>
-    <row r="10" spans="1:33">
+    </row>
+    <row r="10" spans="1:32">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="52"/>
@@ -6732,15 +6722,15 @@
       <c r="J10" s="3"/>
       <c r="K10" s="52"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="73"/>
+      <c r="M10" s="52"/>
       <c r="N10" s="52"/>
       <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
+      <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -6749,12 +6739,11 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
+      <c r="AD10" s="52"/>
       <c r="AE10" s="52"/>
       <c r="AF10" s="52"/>
-      <c r="AG10" s="52"/>
-    </row>
-    <row r="11" spans="1:33">
+    </row>
+    <row r="11" spans="1:32">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="52"/>
@@ -6767,15 +6756,15 @@
       <c r="J11" s="3"/>
       <c r="K11" s="52"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="73"/>
+      <c r="M11" s="52"/>
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
+      <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="55"/>
+      <c r="T11" s="55"/>
+      <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -6784,12 +6773,11 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
+      <c r="AD11" s="52"/>
       <c r="AE11" s="52"/>
       <c r="AF11" s="52"/>
-      <c r="AG11" s="52"/>
-    </row>
-    <row r="12" spans="1:33">
+    </row>
+    <row r="12" spans="1:32">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="52"/>
@@ -6802,15 +6790,15 @@
       <c r="J12" s="3"/>
       <c r="K12" s="52"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="73"/>
+      <c r="M12" s="52"/>
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="55"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -6819,12 +6807,11 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
+      <c r="AD12" s="52"/>
       <c r="AE12" s="52"/>
       <c r="AF12" s="52"/>
-      <c r="AG12" s="52"/>
-    </row>
-    <row r="13" spans="1:33">
+    </row>
+    <row r="13" spans="1:32">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="52"/>
@@ -6837,15 +6824,15 @@
       <c r="J13" s="3"/>
       <c r="K13" s="52"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="73"/>
+      <c r="M13" s="52"/>
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
+      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -6854,12 +6841,11 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
+      <c r="AD13" s="52"/>
       <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
-      <c r="AG13" s="52"/>
-    </row>
-    <row r="14" spans="1:33">
+    </row>
+    <row r="14" spans="1:32">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="52"/>
@@ -6872,15 +6858,15 @@
       <c r="J14" s="3"/>
       <c r="K14" s="52"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="73"/>
+      <c r="M14" s="52"/>
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
+      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -6889,12 +6875,11 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="AD14" s="52"/>
       <c r="AE14" s="52"/>
       <c r="AF14" s="52"/>
-      <c r="AG14" s="52"/>
-    </row>
-    <row r="15" spans="1:33">
+    </row>
+    <row r="15" spans="1:32">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="52"/>
@@ -6907,15 +6892,15 @@
       <c r="J15" s="3"/>
       <c r="K15" s="52"/>
       <c r="L15" s="52"/>
-      <c r="M15" s="73"/>
+      <c r="M15" s="52"/>
       <c r="N15" s="52"/>
       <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
+      <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -6924,12 +6909,11 @@
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
+      <c r="AD15" s="52"/>
       <c r="AE15" s="52"/>
       <c r="AF15" s="52"/>
-      <c r="AG15" s="52"/>
-    </row>
-    <row r="16" spans="1:33">
+    </row>
+    <row r="16" spans="1:32">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="52"/>
@@ -6942,15 +6926,15 @@
       <c r="J16" s="3"/>
       <c r="K16" s="52"/>
       <c r="L16" s="52"/>
-      <c r="M16" s="73"/>
+      <c r="M16" s="52"/>
       <c r="N16" s="52"/>
       <c r="O16" s="52"/>
-      <c r="P16" s="52"/>
+      <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -6959,12 +6943,11 @@
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
+      <c r="AD16" s="52"/>
       <c r="AE16" s="52"/>
       <c r="AF16" s="52"/>
-      <c r="AG16" s="52"/>
-    </row>
-    <row r="17" spans="1:33">
+    </row>
+    <row r="17" spans="1:32">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="52"/>
@@ -6977,15 +6960,15 @@
       <c r="J17" s="3"/>
       <c r="K17" s="52"/>
       <c r="L17" s="52"/>
-      <c r="M17" s="73"/>
+      <c r="M17" s="52"/>
       <c r="N17" s="52"/>
       <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
+      <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -6994,16 +6977,15 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
+      <c r="AD17" s="52"/>
       <c r="AE17" s="52"/>
       <c r="AF17" s="52"/>
-      <c r="AG17" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="X2:X3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -7039,7 +7021,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
@@ -7060,26 +7042,26 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="C3" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="107" t="s">
         <v>123</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>124</v>
       </c>
       <c r="E3" s="107"/>
       <c r="F3" s="107"/>
       <c r="G3" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="9">
         <v>44890</v>
@@ -7182,7 +7164,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="110"/>
       <c r="E3" s="110"/>
@@ -7216,7 +7198,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="110"/>
       <c r="E5" s="110"/>
@@ -7233,7 +7215,7 @@
         <v>2.1</v>
       </c>
       <c r="C6" s="109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="109"/>
       <c r="E6" s="109"/>
@@ -7250,7 +7232,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="109"/>
       <c r="E7" s="109"/>
@@ -7267,7 +7249,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="109" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="109"/>
       <c r="E8" s="109"/>
@@ -7284,7 +7266,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="110" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="110"/>
       <c r="E9" s="110"/>
@@ -7301,7 +7283,7 @@
         <v>3.1</v>
       </c>
       <c r="C10" s="109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="109"/>
       <c r="E10" s="109"/>
@@ -7318,7 +7300,7 @@
         <v>3.2</v>
       </c>
       <c r="C11" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="109"/>
       <c r="E11" s="109"/>
@@ -7335,7 +7317,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="110"/>
       <c r="E12" s="110"/>
@@ -7352,7 +7334,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C13" s="109" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="109"/>
       <c r="E13" s="109"/>
@@ -7369,7 +7351,7 @@
         <v>4.2</v>
       </c>
       <c r="C14" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="109"/>
       <c r="E14" s="109"/>
@@ -7386,7 +7368,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="110" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="110"/>
       <c r="E15" s="110"/>
@@ -7403,7 +7385,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C16" s="109" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D16" s="109"/>
       <c r="E16" s="109"/>
@@ -7519,7 +7501,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>66</v>
@@ -7543,7 +7525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
@@ -7553,7 +7535,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
@@ -7563,7 +7545,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
@@ -7604,13 +7586,13 @@
         <v>65</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>68</v>
@@ -7630,13 +7612,13 @@
         <v>40</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7647,16 +7629,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -7667,16 +7649,16 @@
         <v>17</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7687,16 +7669,16 @@
         <v>17</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7742,16 +7724,16 @@
         <v>65</v>
       </c>
       <c r="B1" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>182</v>
-      </c>
       <c r="E1" s="71" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F1" s="72" t="s">
         <v>70</v>
@@ -7771,16 +7753,16 @@
         <v>18</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7788,19 +7770,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" s="50"/>
     </row>
@@ -7809,19 +7791,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>130</v>
-      </c>
       <c r="D4" s="60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7830,19 +7812,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="60" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>201</v>
-      </c>
       <c r="E5" s="59" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G5" s="50"/>
     </row>
@@ -7898,7 +7880,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="72" t="s">
         <v>71</v>
@@ -7913,10 +7895,10 @@
         <v>74</v>
       </c>
       <c r="G1" s="74" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H1" s="74" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I1" s="72" t="s">
         <v>75</v>
@@ -7928,7 +7910,7 @@
         <v>67</v>
       </c>
       <c r="L1" s="83" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M1" s="79"/>
       <c r="N1" s="79"/>
@@ -7938,25 +7920,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C2" s="81" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E2" s="82">
         <v>1</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G2" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H2" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I2" s="82" t="s">
         <v>41</v>
@@ -7968,7 +7950,7 @@
         <v>49</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M2" s="79"/>
       <c r="N2" s="79"/>
@@ -7978,25 +7960,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C3" s="81" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E3" s="82">
         <v>1</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H3" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I3" s="82" t="s">
         <v>41</v>
@@ -8008,7 +7990,7 @@
         <v>50</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
@@ -8018,25 +8000,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C4" s="81" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
       </c>
       <c r="F4" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H4" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I4" s="82" t="s">
         <v>41</v>
@@ -8048,7 +8030,7 @@
         <v>52</v>
       </c>
       <c r="L4" s="82" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -8056,25 +8038,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C5" s="81" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E5" s="82">
         <v>1</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G5" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I5" s="82" t="s">
         <v>41</v>
@@ -8086,7 +8068,7 @@
         <v>51</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8094,25 +8076,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6" s="81" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E6" s="82">
         <v>1</v>
       </c>
       <c r="F6" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G6" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H6" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I6" s="82" t="s">
         <v>41</v>
@@ -8124,7 +8106,7 @@
         <v>53</v>
       </c>
       <c r="L6" s="82" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8132,25 +8114,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C7" s="81" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E7" s="82">
         <v>1</v>
       </c>
       <c r="F7" s="82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G7" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H7" s="82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I7" s="82" t="s">
         <v>41</v>
@@ -8162,7 +8144,7 @@
         <v>54</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8214,7 +8196,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>77</v>
@@ -8223,13 +8205,13 @@
         <v>68</v>
       </c>
       <c r="E1" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="51" t="s">
         <v>143</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8237,20 +8219,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="47" t="s">
         <v>145</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8332,40 +8314,40 @@
         <v>65</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="F1" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="L1" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="M1" s="56" t="s">
         <v>158</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8406,7 +8388,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8447,7 +8429,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8488,7 +8470,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:13">

</xml_diff>

<commit_message>
Add ECS wave support
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789DDF65-F04F-4CA6-9783-65FACC2EFCEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C15C66-10CB-4EDD-A002-64F3192700CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2298,6 +2298,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2310,9 +2337,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2325,30 +2349,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2367,17 +2367,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5601,22 +5601,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="95"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5628,7 +5628,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="95"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5640,25 +5640,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="95"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="97"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="95"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="87"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="99"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="95"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5666,7 +5666,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="95"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5677,22 +5677,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="92" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5702,31 +5702,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5738,22 +5738,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5763,45 +5763,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="89" t="s">
+      <c r="B20" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5812,50 +5812,60 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="101"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5868,16 +5878,6 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6108,9 +6108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -6121,14 +6119,14 @@
     <col min="5" max="5" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.09765625" style="6" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.19921875" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.8984375" style="6" customWidth="1"/>
     <col min="10" max="10" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.59765625" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.3984375" style="6" customWidth="1"/>
     <col min="17" max="17" width="18.796875" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.59765625" style="6" customWidth="1"/>
@@ -6167,7 +6165,7 @@
       <c r="G1" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="78" t="s">
         <v>172</v>
       </c>
       <c r="I1" s="53" t="s">
@@ -6265,7 +6263,9 @@
       <c r="G2" s="69" t="s">
         <v>227</v>
       </c>
-      <c r="H2" s="70"/>
+      <c r="H2" s="70">
+        <v>1</v>
+      </c>
       <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>188</v>
       </c>
       <c r="N2" s="52"/>
-      <c r="O2" s="52" t="s">
+      <c r="O2" s="84" t="s">
         <v>196</v>
       </c>
       <c r="P2" s="58" t="s">
@@ -6359,7 +6359,9 @@
       <c r="G3" s="69" t="s">
         <v>228</v>
       </c>
-      <c r="H3" s="70"/>
+      <c r="H3" s="70">
+        <v>1</v>
+      </c>
       <c r="I3" s="113"/>
       <c r="J3" s="3" t="s">
         <v>12</v>
@@ -6374,7 +6376,7 @@
         <v>188</v>
       </c>
       <c r="N3" s="52"/>
-      <c r="O3" s="52" t="s">
+      <c r="O3" s="84" t="s">
         <v>196</v>
       </c>
       <c r="P3" s="58" t="s">
@@ -6447,7 +6449,9 @@
       <c r="G4" s="69" t="s">
         <v>229</v>
       </c>
-      <c r="H4" s="70"/>
+      <c r="H4" s="70">
+        <v>1</v>
+      </c>
       <c r="I4" s="73"/>
       <c r="J4" s="73" t="s">
         <v>13</v>
@@ -6464,7 +6468,7 @@
       <c r="N4" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="84" t="s">
         <v>213</v>
       </c>
       <c r="P4" s="58" t="s">
@@ -6525,7 +6529,9 @@
       <c r="G5" s="69" t="s">
         <v>230</v>
       </c>
-      <c r="H5" s="70"/>
+      <c r="H5" s="70">
+        <v>1</v>
+      </c>
       <c r="I5" s="73"/>
       <c r="J5" s="73" t="s">
         <v>13</v>
@@ -6542,7 +6548,7 @@
       <c r="N5" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="84" t="s">
         <v>214</v>
       </c>
       <c r="P5" s="58" t="s">
@@ -6588,7 +6594,7 @@
       <c r="L6" s="52"/>
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
+      <c r="O6" s="84"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -6622,7 +6628,7 @@
       <c r="L7" s="52"/>
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
+      <c r="O7" s="84"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -6656,7 +6662,7 @@
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
+      <c r="O8" s="84"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -6690,7 +6696,7 @@
       <c r="L9" s="52"/>
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
+      <c r="O9" s="84"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -6724,7 +6730,7 @@
       <c r="L10" s="52"/>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
+      <c r="O10" s="84"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -6758,7 +6764,7 @@
       <c r="L11" s="52"/>
       <c r="M11" s="52"/>
       <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
+      <c r="O11" s="84"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
@@ -6792,7 +6798,7 @@
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
       <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="O12" s="84"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
@@ -6826,7 +6832,7 @@
       <c r="L13" s="52"/>
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
+      <c r="O13" s="84"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -6860,7 +6866,7 @@
       <c r="L14" s="52"/>
       <c r="M14" s="52"/>
       <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
+      <c r="O14" s="84"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
@@ -6894,7 +6900,7 @@
       <c r="L15" s="52"/>
       <c r="M15" s="52"/>
       <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
+      <c r="O15" s="84"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
@@ -6928,7 +6934,7 @@
       <c r="L16" s="52"/>
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
+      <c r="O16" s="84"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -6962,7 +6968,7 @@
       <c r="L17" s="52"/>
       <c r="M17" s="52"/>
       <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
+      <c r="O17" s="84"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
@@ -7145,17 +7151,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7163,16 +7169,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7180,16 +7186,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7197,16 +7203,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7214,16 +7220,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7231,16 +7237,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7248,16 +7254,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7265,16 +7271,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="110" t="s">
+      <c r="C9" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7282,16 +7288,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7299,16 +7305,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="110" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="109"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7316,16 +7322,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7333,16 +7339,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="110" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7350,16 +7356,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="110" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="109"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7367,16 +7373,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7384,67 +7390,59 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="109"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="110"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7455,6 +7453,14 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Add Dedicated Host support
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C15C66-10CB-4EDD-A002-64F3192700CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B919BA-EEE7-4B18-83BE-FE983B29CD77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="232">
   <si>
     <t>group01</t>
   </si>
@@ -1584,6 +1584,9 @@
   </si>
   <si>
     <t>ecs-stg</t>
+  </si>
+  <si>
+    <t>Dedicated Host</t>
   </si>
 </sst>
 </file>
@@ -2298,9 +2301,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2325,30 +2352,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2367,17 +2370,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5601,22 +5604,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="87"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="87"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="95"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5628,7 +5631,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="87"/>
+      <c r="E3" s="95"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5640,25 +5643,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="87"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="87"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="95"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="91"/>
+      <c r="C6" s="99"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="87"/>
+      <c r="E6" s="95"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5666,7 +5669,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="87"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5677,22 +5680,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="100" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5702,31 +5705,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5738,22 +5741,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5763,45 +5766,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5812,60 +5815,50 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="100"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="100"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5878,6 +5871,16 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6106,9 +6109,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -6121,29 +6126,30 @@
     <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.19921875" style="6" customWidth="1"/>
     <col min="9" max="9" width="12.8984375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.59765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3984375" style="6" customWidth="1"/>
-    <col min="17" max="17" width="18.796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.59765625" style="6" customWidth="1"/>
-    <col min="19" max="20" width="16.69921875" style="6" customWidth="1"/>
-    <col min="21" max="21" width="12.3984375" style="6" customWidth="1"/>
-    <col min="22" max="22" width="18.796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.69921875" style="6" customWidth="1"/>
-    <col min="24" max="24" width="12.5" style="6" customWidth="1"/>
-    <col min="25" max="25" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="8.796875" style="6"/>
-    <col min="30" max="31" width="8.796875" style="1"/>
-    <col min="32" max="32" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.796875" style="1"/>
+    <col min="10" max="10" width="8.69921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.59765625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.3984375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="18.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.59765625" style="6" customWidth="1"/>
+    <col min="20" max="21" width="16.69921875" style="6" customWidth="1"/>
+    <col min="22" max="22" width="12.3984375" style="6" customWidth="1"/>
+    <col min="23" max="23" width="18.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.69921875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="12.5" style="6" customWidth="1"/>
+    <col min="26" max="26" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="8.796875" style="6"/>
+    <col min="31" max="32" width="8.796875" style="1"/>
+    <col min="33" max="33" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="26.4">
+    <row r="1" spans="1:33" ht="26.4">
       <c r="A1" s="53" t="s">
         <v>65</v>
       </c>
@@ -6171,77 +6177,80 @@
       <c r="I1" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="J1" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="M1" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="N1" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="O1" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="78" t="s">
+      <c r="P1" s="78" t="s">
         <v>173</v>
       </c>
-      <c r="P1" s="78" t="s">
+      <c r="Q1" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="R1" s="78" t="s">
         <v>187</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="S1" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="T1" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="U1" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="V1" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="V1" s="53" t="s">
+      <c r="W1" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="W1" s="53" t="s">
+      <c r="X1" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="Y1" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="Y1" s="78" t="s">
+      <c r="Z1" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" s="78" t="s">
+      <c r="AA1" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="AA1" s="53" t="s">
+      <c r="AB1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="53" t="s">
+      <c r="AE1" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="AE1" s="53" t="s">
+      <c r="AF1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" s="53" t="s">
+      <c r="AG1" s="53" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:33">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6269,75 +6278,76 @@
       <c r="I2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="84"/>
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="L2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="M2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="N2" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="52"/>
+      <c r="P2" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="P2" s="58" t="s">
+      <c r="Q2" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="R2" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="112" t="s">
+      <c r="T2" s="112" t="s">
         <v>223</v>
       </c>
-      <c r="T2" s="55" t="s">
+      <c r="U2" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="V2" s="81" t="s">
+      <c r="W2" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="X2" s="112" t="s">
+      <c r="Y2" s="112" t="s">
         <v>220</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="3">
         <v>50</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="3">
         <v>1024</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AF2" s="3">
         <v>512</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:33">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -6363,71 +6373,72 @@
         <v>1</v>
       </c>
       <c r="I3" s="113"/>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="84"/>
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="L3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="M3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="52" t="s">
+      <c r="N3" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="84" t="s">
+      <c r="O3" s="52"/>
+      <c r="P3" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="P3" s="58" t="s">
+      <c r="Q3" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="Q3" s="81" t="s">
+      <c r="R3" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="S3" s="113"/>
-      <c r="T3" s="55" t="s">
+      <c r="T3" s="113"/>
+      <c r="U3" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="U3" s="75" t="s">
+      <c r="V3" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="81" t="s">
+      <c r="W3" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="X3" s="113"/>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="113"/>
+      <c r="Z3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>50</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>1024</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>512</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:33">
       <c r="A4" s="73">
         <v>3</v>
       </c>
@@ -6453,65 +6464,66 @@
         <v>1</v>
       </c>
       <c r="I4" s="73"/>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="84"/>
+      <c r="K4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="52" t="s">
+      <c r="L4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="52" t="s">
+      <c r="M4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="N4" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="N4" s="52" t="s">
+      <c r="O4" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="84" t="s">
+      <c r="P4" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="P4" s="58" t="s">
+      <c r="Q4" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="Q4" s="81" t="s">
+      <c r="R4" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="S4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="73"/>
       <c r="T4" s="73"/>
       <c r="U4" s="73"/>
       <c r="V4" s="73"/>
       <c r="W4" s="73"/>
       <c r="X4" s="73"/>
-      <c r="Y4" s="73" t="s">
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="73">
+      <c r="AA4" s="73">
         <v>100</v>
       </c>
-      <c r="AA4" s="73" t="s">
+      <c r="AB4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="73">
+      <c r="AC4" s="73">
         <v>512</v>
       </c>
-      <c r="AC4" s="73" t="s">
+      <c r="AD4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="AD4" s="73" t="s">
+      <c r="AE4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="73">
+      <c r="AF4" s="73">
         <v>512</v>
       </c>
-      <c r="AF4" s="73" t="s">
+      <c r="AG4" s="73" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:33">
       <c r="A5" s="73">
         <v>4</v>
       </c>
@@ -6533,53 +6545,56 @@
         <v>1</v>
       </c>
       <c r="I5" s="73"/>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="L5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="M5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="52" t="s">
+      <c r="N5" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="O5" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="O5" s="84" t="s">
+      <c r="P5" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="P5" s="58" t="s">
+      <c r="Q5" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="Q5" s="81" t="s">
+      <c r="R5" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="R5" s="73" t="s">
+      <c r="S5" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="S5" s="73"/>
       <c r="T5" s="73"/>
       <c r="U5" s="73"/>
       <c r="V5" s="73"/>
       <c r="W5" s="73"/>
       <c r="X5" s="73"/>
-      <c r="Y5" s="73" t="s">
+      <c r="Y5" s="73"/>
+      <c r="Z5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="Z5" s="73">
+      <c r="AA5" s="73">
         <v>100</v>
       </c>
-      <c r="AA5" s="73"/>
       <c r="AB5" s="73"/>
       <c r="AC5" s="73"/>
-      <c r="AD5" s="52"/>
+      <c r="AD5" s="73"/>
       <c r="AE5" s="52"/>
       <c r="AF5" s="52"/>
-    </row>
-    <row r="6" spans="1:32">
+      <c r="AG5" s="52"/>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="52"/>
@@ -6589,18 +6604,18 @@
       <c r="G6" s="69"/>
       <c r="H6" s="70"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="52"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="52"/>
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="3"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="84"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="55"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
@@ -6609,11 +6624,12 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
-      <c r="AD6" s="52"/>
+      <c r="AD6" s="3"/>
       <c r="AE6" s="52"/>
       <c r="AF6" s="52"/>
-    </row>
-    <row r="7" spans="1:32">
+      <c r="AG6" s="52"/>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="52"/>
@@ -6623,18 +6639,18 @@
       <c r="G7" s="69"/>
       <c r="H7" s="70"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="52"/>
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="3"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="84"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="55"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -6643,11 +6659,12 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="52"/>
+      <c r="AD7" s="3"/>
       <c r="AE7" s="52"/>
       <c r="AF7" s="52"/>
-    </row>
-    <row r="8" spans="1:32">
+      <c r="AG7" s="52"/>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="52"/>
@@ -6657,18 +6674,18 @@
       <c r="G8" s="69"/>
       <c r="H8" s="70"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="3"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="84"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="55"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
@@ -6677,11 +6694,12 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="52"/>
+      <c r="AD8" s="3"/>
       <c r="AE8" s="52"/>
       <c r="AF8" s="52"/>
-    </row>
-    <row r="9" spans="1:32">
+      <c r="AG8" s="52"/>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="52"/>
@@ -6691,18 +6709,18 @@
       <c r="G9" s="69"/>
       <c r="H9" s="70"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="52"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="52"/>
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="3"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="84"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="55"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -6711,11 +6729,12 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
-      <c r="AD9" s="52"/>
+      <c r="AD9" s="3"/>
       <c r="AE9" s="52"/>
       <c r="AF9" s="52"/>
-    </row>
-    <row r="10" spans="1:32">
+      <c r="AG9" s="52"/>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="52"/>
@@ -6725,18 +6744,18 @@
       <c r="G10" s="69"/>
       <c r="H10" s="70"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="52"/>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="3"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="84"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="55"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -6745,11 +6764,12 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
-      <c r="AD10" s="52"/>
+      <c r="AD10" s="3"/>
       <c r="AE10" s="52"/>
       <c r="AF10" s="52"/>
-    </row>
-    <row r="11" spans="1:32">
+      <c r="AG10" s="52"/>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="52"/>
@@ -6759,18 +6779,18 @@
       <c r="G11" s="69"/>
       <c r="H11" s="70"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="52"/>
       <c r="M11" s="52"/>
       <c r="N11" s="52"/>
-      <c r="O11" s="84"/>
-      <c r="P11" s="3"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="84"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="55"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -6779,11 +6799,12 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
-      <c r="AD11" s="52"/>
+      <c r="AD11" s="3"/>
       <c r="AE11" s="52"/>
       <c r="AF11" s="52"/>
-    </row>
-    <row r="12" spans="1:32">
+      <c r="AG11" s="52"/>
+    </row>
+    <row r="12" spans="1:33">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="52"/>
@@ -6793,18 +6814,18 @@
       <c r="G12" s="69"/>
       <c r="H12" s="70"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="52"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
       <c r="N12" s="52"/>
-      <c r="O12" s="84"/>
-      <c r="P12" s="3"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="84"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="55"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -6813,11 +6834,12 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
-      <c r="AD12" s="52"/>
+      <c r="AD12" s="3"/>
       <c r="AE12" s="52"/>
       <c r="AF12" s="52"/>
-    </row>
-    <row r="13" spans="1:32">
+      <c r="AG12" s="52"/>
+    </row>
+    <row r="13" spans="1:33">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="52"/>
@@ -6827,18 +6849,18 @@
       <c r="G13" s="69"/>
       <c r="H13" s="70"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="52"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="52"/>
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
-      <c r="O13" s="84"/>
-      <c r="P13" s="3"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="84"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="55"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -6847,11 +6869,12 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
-      <c r="AD13" s="52"/>
+      <c r="AD13" s="3"/>
       <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
-    </row>
-    <row r="14" spans="1:32">
+      <c r="AG13" s="52"/>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="52"/>
@@ -6861,18 +6884,18 @@
       <c r="G14" s="69"/>
       <c r="H14" s="70"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="52"/>
+      <c r="J14" s="84"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="52"/>
       <c r="M14" s="52"/>
       <c r="N14" s="52"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="3"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="84"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="55"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -6881,11 +6904,12 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
-      <c r="AD14" s="52"/>
+      <c r="AD14" s="3"/>
       <c r="AE14" s="52"/>
       <c r="AF14" s="52"/>
-    </row>
-    <row r="15" spans="1:32">
+      <c r="AG14" s="52"/>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="52"/>
@@ -6895,18 +6919,18 @@
       <c r="G15" s="69"/>
       <c r="H15" s="70"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="52"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="52"/>
       <c r="M15" s="52"/>
       <c r="N15" s="52"/>
-      <c r="O15" s="84"/>
-      <c r="P15" s="3"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="84"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="55"/>
-      <c r="U15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="55"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -6915,11 +6939,12 @@
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
-      <c r="AD15" s="52"/>
+      <c r="AD15" s="3"/>
       <c r="AE15" s="52"/>
       <c r="AF15" s="52"/>
-    </row>
-    <row r="16" spans="1:32">
+      <c r="AG15" s="52"/>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="52"/>
@@ -6929,18 +6954,18 @@
       <c r="G16" s="69"/>
       <c r="H16" s="70"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="52"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="52"/>
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="3"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="84"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="55"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -6949,11 +6974,12 @@
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
-      <c r="AD16" s="52"/>
+      <c r="AD16" s="3"/>
       <c r="AE16" s="52"/>
       <c r="AF16" s="52"/>
-    </row>
-    <row r="17" spans="1:32">
+      <c r="AG16" s="52"/>
+    </row>
+    <row r="17" spans="1:33">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="52"/>
@@ -6963,18 +6989,18 @@
       <c r="G17" s="69"/>
       <c r="H17" s="70"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="52"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="52"/>
       <c r="M17" s="52"/>
       <c r="N17" s="52"/>
-      <c r="O17" s="84"/>
-      <c r="P17" s="3"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="84"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="55"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -6983,15 +7009,16 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
-      <c r="AD17" s="52"/>
+      <c r="AD17" s="3"/>
       <c r="AE17" s="52"/>
       <c r="AF17" s="52"/>
+      <c r="AG17" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="Y2:Y3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -7151,17 +7178,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7169,16 +7196,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7186,16 +7213,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7203,16 +7230,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7220,16 +7247,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7237,16 +7264,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7254,16 +7281,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7271,16 +7298,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7288,16 +7315,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="110" t="s">
+      <c r="C10" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7305,16 +7332,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7322,16 +7349,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="109"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7339,16 +7366,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7356,16 +7383,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7373,16 +7400,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7390,59 +7417,67 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="110" t="s">
+      <c r="C16" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="109"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7453,14 +7488,6 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix different secgroups for different NICs
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B919BA-EEE7-4B18-83BE-FE983B29CD77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5886C2C9-C225-4C52-A5DF-9789EFAFFC39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="233">
   <si>
     <t>group01</t>
   </si>
@@ -1587,6 +1587,9 @@
   </si>
   <si>
     <t>Dedicated Host</t>
+  </si>
+  <si>
+    <t>dev-sg001</t>
   </si>
 </sst>
 </file>
@@ -2301,6 +2304,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2313,9 +2343,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2328,30 +2355,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2370,17 +2373,17 @@
     <xf numFmtId="0" fontId="41" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5604,22 +5607,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.1" customHeight="1">
       <c r="A1" s="15"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="95"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5631,7 +5634,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="95"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
@@ -5643,25 +5646,25 @@
         <v>45024</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="95"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="375" customHeight="1">
-      <c r="A5" s="97"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="95"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="87"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="99"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="95"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
@@ -5669,7 +5672,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="95"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1">
@@ -5680,22 +5683,22 @@
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="92" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="25"/>
@@ -5705,31 +5708,31 @@
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
@@ -5741,22 +5744,22 @@
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
     </row>
     <row r="18" spans="1:5" ht="15.6">
       <c r="A18" s="28"/>
@@ -5766,45 +5769,45 @@
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="89" t="s">
+      <c r="B20" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" ht="14.4">
@@ -5815,50 +5818,60 @@
       <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20.399999999999999">
-      <c r="A24" s="92"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1">
       <c r="A25" s="33"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="101"/>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1">
       <c r="A26" s="33"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1">
       <c r="A27" s="33"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="33"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="33"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E7"/>
@@ -5871,16 +5884,6 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6112,7 +6115,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6314,7 +6317,7 @@
         <v>198</v>
       </c>
       <c r="W2" s="81" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>218</v>
@@ -6407,7 +6410,7 @@
         <v>198</v>
       </c>
       <c r="W3" s="81" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>219</v>
@@ -7178,17 +7181,17 @@
       <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
@@ -7196,16 +7199,16 @@
       <c r="B3" s="40">
         <v>1</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="14.4">
@@ -7213,16 +7216,16 @@
       <c r="B4" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
       <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
@@ -7230,16 +7233,16 @@
       <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
       <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="14.4">
@@ -7247,16 +7250,16 @@
       <c r="B6" s="42">
         <v>2.1</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="110" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="14.4">
@@ -7264,16 +7267,16 @@
       <c r="B7" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
       <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="14.4">
@@ -7281,16 +7284,16 @@
       <c r="B8" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
       <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
@@ -7298,16 +7301,16 @@
       <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="110" t="s">
+      <c r="C9" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
       <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
@@ -7315,16 +7318,16 @@
       <c r="B10" s="42">
         <v>3.1</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="110" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="14.4">
@@ -7332,16 +7335,16 @@
       <c r="B11" s="42">
         <v>3.2</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="110" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="109"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
@@ -7349,16 +7352,16 @@
       <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
       <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:11" ht="14.4">
@@ -7366,16 +7369,16 @@
       <c r="B13" s="42">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="110" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
       <c r="K13" s="41"/>
     </row>
     <row r="14" spans="1:11" ht="14.4">
@@ -7383,16 +7386,16 @@
       <c r="B14" s="42">
         <v>4.2</v>
       </c>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="110" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="109"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
       <c r="K14" s="41"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -7400,16 +7403,16 @@
       <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" ht="14.4">
@@ -7417,67 +7420,59 @@
       <c r="B16" s="42">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="109"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="110"/>
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="110"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="39"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="39"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
       <c r="K19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C19:J19"/>
     <mergeCell ref="C8:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -7488,6 +7483,14 @@
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C13:J13"/>
     <mergeCell ref="C14:J14"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Small cosmetic updates in the LLD
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Terraform\lld-to-terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5886C2C9-C225-4C52-A5DF-9789EFAFFC39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3BD129B-51FD-4E89-BA98-A3CC370F5552}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="5580" windowHeight="5016" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,6 +476,7 @@
     <definedName name="WET">[2]menus!$G$2:$G$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -765,10 +766,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>01</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Date</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -1590,6 +1587,9 @@
   </si>
   <si>
     <t>dev-sg001</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
@@ -5618,7 +5618,7 @@
     <row r="2" spans="1:6" ht="111.6" customHeight="1">
       <c r="A2" s="18"/>
       <c r="B2" s="88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="88"/>
       <c r="D2" s="88"/>
@@ -5631,7 +5631,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>21</v>
+        <v>232</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="87"/>
@@ -5640,7 +5640,7 @@
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="21">
         <v>45024</v>
@@ -5660,7 +5660,7 @@
     <row r="6" spans="1:6" ht="130.35" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="91"/>
       <c r="D6" s="18"/>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="92" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" s="92"/>
       <c r="C9" s="92"/>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1">
       <c r="A10" s="93" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.9" customHeight="1">
       <c r="A12" s="92" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="92"/>
       <c r="C12" s="92"/>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
       <c r="A13" s="85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="85"/>
       <c r="C13" s="85"/>
@@ -5727,7 +5727,7 @@
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1">
       <c r="A14" s="85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="85"/>
       <c r="C14" s="85"/>
@@ -5736,7 +5736,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
@@ -5745,7 +5745,7 @@
     </row>
     <row r="16" spans="1:6" ht="72" customHeight="1">
       <c r="A16" s="85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="85"/>
       <c r="C16" s="85"/>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="17" spans="1:5" ht="58.5" customHeight="1">
       <c r="A17" s="85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="85"/>
       <c r="C17" s="85"/>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1">
       <c r="A19" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="97"/>
       <c r="C19" s="97"/>
@@ -5779,10 +5779,10 @@
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1">
       <c r="A20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="85" t="s">
         <v>32</v>
-      </c>
-      <c r="B20" s="85" t="s">
-        <v>33</v>
       </c>
       <c r="C20" s="85"/>
       <c r="D20" s="85"/>
@@ -5790,10 +5790,10 @@
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1">
       <c r="A21" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="98" t="s">
         <v>34</v>
-      </c>
-      <c r="B21" s="98" t="s">
-        <v>35</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
@@ -5801,10 +5801,10 @@
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1">
       <c r="A22" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="99" t="s">
         <v>36</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>37</v>
       </c>
       <c r="C22" s="99"/>
       <c r="D22" s="99"/>
@@ -5903,13 +5903,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3C65F-293E-4583-9953-24F4023C82CC}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.59765625" style="46" customWidth="1"/>
     <col min="3" max="3" width="21.59765625" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.796875" style="46" customWidth="1"/>
@@ -5922,37 +5920,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="G1" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>164</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>169</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5960,14 +5958,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>166</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>167</v>
       </c>
       <c r="F2" s="59">
         <v>30</v>
@@ -5988,9 +5986,7 @@
       <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="58"/>
@@ -6019,13 +6015,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9165AE6A-6DD8-413C-988C-A8ABE320BD6D}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.296875" customWidth="1"/>
     <col min="3" max="3" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.296875" bestFit="1" customWidth="1"/>
@@ -6035,37 +6029,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="F1" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="51" t="s">
         <v>83</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -6084,9 +6078,7 @@
       <c r="K2" s="45"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="11"/>
@@ -6114,13 +6106,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
@@ -6154,103 +6144,103 @@
   <sheetData>
     <row r="1" spans="1:33" ht="26.4">
       <c r="A1" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C1" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>103</v>
       </c>
       <c r="E1" s="78" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="J1" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="I1" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="53" t="s">
-        <v>231</v>
-      </c>
-      <c r="K1" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="M1" s="78" t="s">
+      <c r="Q1" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="R1" s="78" t="s">
+        <v>186</v>
+      </c>
+      <c r="S1" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="78" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q1" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="R1" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="S1" s="53" t="s">
+      <c r="U1" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="W1" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y1" s="53" t="s">
-        <v>186</v>
-      </c>
-      <c r="Z1" s="78" t="s">
+      <c r="AA1" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="78" t="s">
+      <c r="AB1" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AC1" s="53" t="s">
+      <c r="AD1" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="AD1" s="53" t="s">
+      <c r="AE1" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="AE1" s="53" t="s">
+      <c r="AF1" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="AF1" s="53" t="s">
+      <c r="AG1" s="53" t="s">
         <v>99</v>
-      </c>
-      <c r="AG1" s="53" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -6258,22 +6248,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H2" s="70">
         <v>1</v>
@@ -6292,38 +6282,38 @@
         <v>10</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O2" s="52"/>
       <c r="P2" s="84" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="Q2" s="58" t="s">
+      <c r="R2" s="81" t="s">
+        <v>209</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="T2" s="112" t="s">
+        <v>222</v>
+      </c>
+      <c r="U2" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="R2" s="81" t="s">
-        <v>210</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="T2" s="112" t="s">
-        <v>223</v>
-      </c>
-      <c r="U2" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="W2" s="81" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Y2" s="112" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>7</v>
@@ -6355,22 +6345,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H3" s="70">
         <v>1</v>
@@ -6387,33 +6377,33 @@
         <v>10</v>
       </c>
       <c r="N3" s="52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O3" s="52"/>
       <c r="P3" s="84" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q3" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="Q3" s="58" t="s">
-        <v>197</v>
-      </c>
       <c r="R3" s="81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T3" s="113"/>
       <c r="U3" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="W3" s="81" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y3" s="113"/>
       <c r="Z3" s="3" t="s">
@@ -6446,22 +6436,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="73" t="s">
-        <v>105</v>
-      </c>
       <c r="E4" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H4" s="70">
         <v>1</v>
@@ -6478,19 +6468,19 @@
         <v>11</v>
       </c>
       <c r="N4" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="O4" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="O4" s="52" t="s">
-        <v>189</v>
-      </c>
       <c r="P4" s="84" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q4" s="58" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="R4" s="81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S4" s="73" t="s">
         <v>6</v>
@@ -6531,18 +6521,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="73" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H5" s="70">
         <v>1</v>
@@ -6561,22 +6551,22 @@
         <v>11</v>
       </c>
       <c r="N5" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="O5" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="O5" s="52" t="s">
-        <v>189</v>
-      </c>
       <c r="P5" s="84" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q5" s="58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R5" s="81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S5" s="73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T5" s="73"/>
       <c r="U5" s="73"/>
@@ -7038,9 +7028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3783224E-E7A7-46DD-8162-756DEBD8067E}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
@@ -7057,7 +7045,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="104"/>
       <c r="D1" s="104"/>
@@ -7078,26 +7066,26 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="C3" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="107" t="s">
         <v>122</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>123</v>
       </c>
       <c r="E3" s="107"/>
       <c r="F3" s="107"/>
       <c r="G3" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="9">
         <v>44890</v>
@@ -7182,7 +7170,7 @@
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
       <c r="B2" s="108" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="108"/>
       <c r="D2" s="108"/>
@@ -7200,7 +7188,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="109"/>
       <c r="E3" s="109"/>
@@ -7217,7 +7205,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="110"/>
       <c r="E4" s="110"/>
@@ -7234,7 +7222,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
@@ -7251,7 +7239,7 @@
         <v>2.1</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
@@ -7268,7 +7256,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="110"/>
       <c r="E7" s="110"/>
@@ -7285,7 +7273,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C8" s="110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="110"/>
       <c r="E8" s="110"/>
@@ -7302,7 +7290,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="109"/>
       <c r="E9" s="109"/>
@@ -7319,7 +7307,7 @@
         <v>3.1</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="110"/>
       <c r="E10" s="110"/>
@@ -7336,7 +7324,7 @@
         <v>3.2</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="110"/>
       <c r="E11" s="110"/>
@@ -7353,7 +7341,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="109"/>
       <c r="E12" s="109"/>
@@ -7370,7 +7358,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C13" s="110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="110"/>
       <c r="E13" s="110"/>
@@ -7387,7 +7375,7 @@
         <v>4.2</v>
       </c>
       <c r="C14" s="110" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" s="110"/>
       <c r="E14" s="110"/>
@@ -7404,7 +7392,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="109"/>
       <c r="E15" s="109"/>
@@ -7421,7 +7409,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C16" s="110" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="110"/>
       <c r="E16" s="110"/>
@@ -7519,13 +7507,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABE4133-68EE-4AE2-AF8E-B7881ADA2847}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="61"/>
+    <col min="1" max="1" width="4.5" style="61" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.796875" style="61" customWidth="1"/>
     <col min="3" max="3" width="32.69921875" style="61" customWidth="1"/>
     <col min="4" max="4" width="57.5" style="61" customWidth="1"/>
@@ -7534,16 +7520,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="43" customFormat="1">
       <c r="A1" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>174</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>66</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="43" customFormat="1">
@@ -7551,7 +7537,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -7561,7 +7547,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
@@ -7571,7 +7557,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
@@ -7581,7 +7567,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
@@ -7602,13 +7588,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF70B82-AD66-493E-91C9-92B94A95EEFB}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="76"/>
+    <col min="1" max="1" width="4.5" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.796875" style="76" customWidth="1"/>
     <col min="3" max="3" width="13.59765625" style="76" customWidth="1"/>
     <col min="4" max="4" width="15.3984375" style="5" customWidth="1"/>
@@ -7619,22 +7603,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="D1" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="72" t="s">
-        <v>177</v>
-      </c>
       <c r="E1" s="56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7645,16 +7629,16 @@
         <v>17</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7665,16 +7649,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -7685,16 +7669,16 @@
         <v>17</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7705,16 +7689,16 @@
         <v>17</v>
       </c>
       <c r="C5" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7741,12 +7725,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B2074E-480A-4904-B9AE-9A861A42FF00}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" customWidth="1"/>
     <col min="3" max="3" width="14.19921875" style="46" customWidth="1"/>
     <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
@@ -7757,25 +7740,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="72" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="71" t="s">
-        <v>177</v>
-      </c>
       <c r="F1" s="72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7783,22 +7766,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="13.2">
@@ -7806,19 +7789,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="50"/>
     </row>
@@ -7827,19 +7810,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>129</v>
-      </c>
       <c r="D4" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G4" s="50"/>
     </row>
@@ -7848,19 +7831,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="63" t="s">
         <v>216</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>217</v>
       </c>
       <c r="G5" s="50"/>
     </row>
@@ -7889,13 +7872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEFA34F-B9F8-479A-9FFB-8E39D313520D}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="76"/>
+    <col min="1" max="1" width="4.5" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.796875" style="76" customWidth="1"/>
     <col min="3" max="3" width="19.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.296875" style="6" bestFit="1" customWidth="1"/>
@@ -7913,40 +7894,40 @@
   <sheetData>
     <row r="1" spans="1:14" s="80" customFormat="1">
       <c r="A1" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="E1" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="F1" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="G1" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="74" t="s">
-        <v>206</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="72" t="s">
+      <c r="J1" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="72" t="s">
-        <v>76</v>
-      </c>
       <c r="K1" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L1" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M1" s="79"/>
       <c r="N1" s="79"/>
@@ -7956,37 +7937,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="82" t="s">
         <v>203</v>
-      </c>
-      <c r="C2" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>204</v>
       </c>
       <c r="E2" s="82">
         <v>1</v>
       </c>
       <c r="F2" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H2" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I2" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M2" s="79"/>
       <c r="N2" s="79"/>
@@ -7996,37 +7977,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E3" s="82">
         <v>1</v>
       </c>
       <c r="F3" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H3" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I3" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" s="82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="82" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L3" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
@@ -8036,37 +8017,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="82" t="s">
         <v>203</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>204</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
       </c>
       <c r="F4" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H4" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I4" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" s="82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L4" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -8074,37 +8055,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5" s="82">
         <v>1</v>
       </c>
       <c r="F5" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G5" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H5" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K5" s="82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8112,37 +8093,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="82" t="s">
         <v>203</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="82" t="s">
-        <v>204</v>
       </c>
       <c r="E6" s="82">
         <v>1</v>
       </c>
       <c r="F6" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G6" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H6" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I6" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L6" s="82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8150,37 +8131,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E7" s="82">
         <v>1</v>
       </c>
       <c r="F7" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G7" s="82" t="s">
-        <v>209</v>
-      </c>
       <c r="H7" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I7" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" s="82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="82" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8213,13 +8194,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0637E39-84C5-4EA8-B9B1-08763F5A9279}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="46"/>
+    <col min="1" max="1" width="4.8984375" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.3984375" style="46" customWidth="1"/>
     <col min="3" max="4" width="22.296875" style="46" customWidth="1"/>
     <col min="5" max="5" width="30" style="46" customWidth="1"/>
@@ -8229,25 +8208,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8255,20 +8234,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="47" t="s">
         <v>144</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8294,9 +8273,7 @@
       <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="47">
-        <v>4</v>
-      </c>
+      <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -8324,13 +8301,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABE9F15-FC5E-4784-8FD8-D852E6A9C381}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="3.8984375" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.8984375" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.3984375" style="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.59765625" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.3984375" style="46" customWidth="1"/>
@@ -8347,43 +8322,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="F1" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="L1" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="M1" s="56" t="s">
         <v>157</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8391,10 +8366,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="47">
         <v>1</v>
@@ -8403,19 +8378,19 @@
         <v>0</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="47">
         <v>0</v>
       </c>
       <c r="I2" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="47" t="s">
         <v>62</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>63</v>
       </c>
       <c r="K2" s="47">
         <v>1</v>
@@ -8424,7 +8399,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8432,10 +8407,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="47">
         <v>4</v>
@@ -8444,19 +8419,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" s="47">
         <v>0</v>
       </c>
       <c r="I3" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="47" t="s">
         <v>62</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>63</v>
       </c>
       <c r="K3" s="47">
         <v>1</v>
@@ -8465,7 +8440,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8473,10 +8448,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="47">
         <v>2</v>
@@ -8485,19 +8460,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="47">
         <v>0</v>
       </c>
       <c r="I4" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="47" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="47" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="47">
         <v>1</v>
@@ -8506,7 +8481,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:13">

</xml_diff>

<commit_message>
Add SNAT rule support
</commit_message>
<xml_diff>
--- a/LLD.xlsx
+++ b/LLD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96659DB-F10F-4B30-A93A-7736F1481A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CB93CE-05F2-444B-85BE-55AD557B6393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2232" windowWidth="23256" windowHeight="13176" tabRatio="916" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="2232" windowWidth="23256" windowHeight="13176" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="9" r:id="rId1"/>
@@ -864,7 +864,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="254">
   <si>
     <t>group01</t>
   </si>
@@ -1760,9 +1760,6 @@
     <t>EIP Name</t>
   </si>
   <si>
-    <t>eip-dev01</t>
-  </si>
-  <si>
     <t>Charge Mode</t>
   </si>
   <si>
@@ -1817,7 +1814,13 @@
     <t>DNAT Subnet Name</t>
   </si>
   <si>
-    <t>eip-stg</t>
+    <t>SNAT</t>
+  </si>
+  <si>
+    <t>eip-dev01-inbound</t>
+  </si>
+  <si>
+    <t>eip-dev01-outbound</t>
   </si>
 </sst>
 </file>
@@ -5841,7 +5844,7 @@
   </sheetPr>
   <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
@@ -6151,15 +6154,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A09F4C0-732E-4565-BC52-69096A866992}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.5" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.796875" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.3984375" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="6" bestFit="1" customWidth="1"/>
@@ -6167,66 +6170,62 @@
     <col min="9" max="9" width="18.296875" style="6" customWidth="1"/>
     <col min="10" max="10" width="16.3984375" style="6" customWidth="1"/>
     <col min="11" max="11" width="21" style="6" customWidth="1"/>
-    <col min="12" max="12" width="15.296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.796875" style="1"/>
-    <col min="15" max="16384" width="8.796875" style="5"/>
+    <col min="12" max="13" width="8.796875" style="1"/>
+    <col min="14" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="86" customFormat="1">
+    <row r="1" spans="1:13" s="86" customFormat="1">
       <c r="A1" s="91" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D1" s="89" t="s">
         <v>232</v>
       </c>
       <c r="E1" s="89" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F1" s="88" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="88" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="88" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="88" t="s">
-        <v>251</v>
-      </c>
-      <c r="H1" s="88" t="s">
-        <v>250</v>
-      </c>
-      <c r="I1" s="88" t="s">
-        <v>246</v>
-      </c>
       <c r="J1" s="88" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K1" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="88" t="s">
-        <v>212</v>
-      </c>
+      <c r="L1" s="87"/>
       <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-    </row>
-    <row r="2" spans="1:14" s="86" customFormat="1">
+    </row>
+    <row r="2" spans="1:13" s="86" customFormat="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="E2" s="84" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="84">
         <v>80</v>
@@ -6242,29 +6241,35 @@
       </c>
       <c r="J2" s="84"/>
       <c r="K2" s="84"/>
-      <c r="L2" s="84" t="s">
-        <v>210</v>
-      </c>
+      <c r="L2" s="87"/>
       <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-    </row>
-    <row r="3" spans="1:14" s="86" customFormat="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="84"/>
+    </row>
+    <row r="3" spans="1:13" s="86" customFormat="1">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>253</v>
+      </c>
       <c r="E3" s="84"/>
       <c r="F3" s="84"/>
       <c r="G3" s="84"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
+      <c r="J3" s="84" t="s">
+        <v>222</v>
+      </c>
       <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
+      <c r="L3" s="87"/>
       <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6276,9 +6281,8 @@
       <c r="I4" s="84"/>
       <c r="J4" s="84"/>
       <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -6290,9 +6294,8 @@
       <c r="I5" s="84"/>
       <c r="J5" s="84"/>
       <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -6304,9 +6307,8 @@
       <c r="I6" s="84"/>
       <c r="J6" s="84"/>
       <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -6318,9 +6320,8 @@
       <c r="I7" s="84"/>
       <c r="J7" s="84"/>
       <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="4"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6332,7 +6333,6 @@
       <c r="I8" s="84"/>
       <c r="J8" s="84"/>
       <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -6850,8 +6850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -8028,7 +8028,7 @@
         <v>2.4</v>
       </c>
       <c r="C9" s="116" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D9" s="116"/>
       <c r="E9" s="116"/>
@@ -8942,14 +8942,14 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.796875" style="76" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.09765625" style="5" customWidth="1"/>
     <col min="4" max="5" width="12.59765625" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.296875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.796875" style="1"/>
@@ -8967,10 +8967,10 @@
         <v>232</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F1" s="85" t="s">
         <v>212</v>
@@ -8986,10 +8986,10 @@
         <v>200</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E2" s="82">
         <v>100</v>
@@ -9001,16 +9001,24 @@
       <c r="H2" s="79"/>
     </row>
     <row r="3" spans="1:8" s="80" customFormat="1">
-      <c r="A3" s="81"/>
+      <c r="A3" s="81">
+        <v>2</v>
+      </c>
       <c r="B3" s="81" t="s">
         <v>200</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>252</v>
-      </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
+        <v>253</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="82">
+        <v>100</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>210</v>
+      </c>
       <c r="G3" s="79"/>
       <c r="H3" s="79"/>
     </row>
@@ -9091,7 +9099,7 @@
         <v>172</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D1" s="89" t="s">
         <v>173</v>
@@ -9100,10 +9108,10 @@
         <v>176</v>
       </c>
       <c r="F1" s="89" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G1" s="88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H1" s="88" t="s">
         <v>231</v>
@@ -9122,7 +9130,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D2" s="84" t="s">
         <v>210</v>
@@ -9135,7 +9143,7 @@
       </c>
       <c r="G2" s="84"/>
       <c r="H2" s="84" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I2" s="84" t="s">
         <v>210</v>

</xml_diff>